<commit_message>
Updated data analysis 25Nov2024
</commit_message>
<xml_diff>
--- a/data/gint export_310724_su.xlsx
+++ b/data/gint export_310724_su.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://geoquip-my.sharepoint.com/personal/yu_wong_geoquip-marine_com/Documents/Documents/Side projects/SHANSEP/Data analysis/data/raw gINT/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://geoquip-my.sharepoint.com/personal/yu_wong_geoquip-marine_com/Documents/Documents/Side projects/SHANSEP/Data analysis/github/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="17" documentId="13_ncr:1_{53DC8D34-75BB-4057-A3EE-40C8B1B84AF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{12F72591-9EA8-4170-8D5B-E8B98382D68E}"/>
+  <xr:revisionPtr revIDLastSave="18" documentId="13_ncr:1_{53DC8D34-75BB-4057-A3EE-40C8B1B84AF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1BA53786-2F76-4AAD-BA7E-2D198C31B39E}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{8E2F55F8-1706-435F-AA5E-3513E323C5DC}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{8E2F55F8-1706-435F-AA5E-3513E323C5DC}"/>
   </bookViews>
   <sheets>
     <sheet name="LPEN" sheetId="2" r:id="rId1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9815" uniqueCount="651">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9814" uniqueCount="651">
   <si>
     <t>PointID</t>
   </si>
@@ -2423,8 +2423,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{700929CE-F83B-4E3F-BCB5-3A5C61A5DD86}">
   <dimension ref="A1:S476"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -29487,8 +29487,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95CD5170-D518-402A-8D22-EAB1380F2A22}">
   <dimension ref="A1:W62"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -29739,7 +29739,7 @@
         <v>329</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>320</v>
+        <v>329</v>
       </c>
       <c r="N4" s="3" t="s">
         <v>23</v>
@@ -30088,9 +30088,6 @@
       </c>
       <c r="I10" s="3" t="s">
         <v>326</v>
-      </c>
-      <c r="J10" s="3" t="s">
-        <v>329</v>
       </c>
       <c r="K10" s="3" t="s">
         <v>320</v>
@@ -46090,7 +46087,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83DF99EE-FB3B-4B36-A107-D3BD802F3E50}">
   <dimension ref="A1:AP74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AA1" workbookViewId="0">
+    <sheetView topLeftCell="AA1" workbookViewId="0">
       <selection activeCell="AM4" sqref="AM4"/>
     </sheetView>
   </sheetViews>
@@ -46385,7 +46382,7 @@
         <v>0.997</v>
       </c>
       <c r="AP2" t="str" cm="1">
-        <f t="array" ref="AP2">_xlfn.XLOOKUP(1, (A2=TREG!A:A)*(CU!F2=TREG!F:F), TREG!J:J)</f>
+        <f t="array" aca="1" ref="AP2" ca="1">_xlfn.XLOOKUP(1, (A2=TREG!A:A)*(CU!F2=TREG!F:F), TREG!J:J)</f>
         <v>CAUC</v>
       </c>
     </row>
@@ -46508,7 +46505,7 @@
         <v>0.70499999999999996</v>
       </c>
       <c r="AP3" t="str" cm="1">
-        <f t="array" ref="AP3">_xlfn.XLOOKUP(1, (A3=TREG!A:A)*(CU!F3=TREG!F:F), TREG!J:J)</f>
+        <f t="array" aca="1" ref="AP3" ca="1">_xlfn.XLOOKUP(1, (A3=TREG!A:A)*(CU!F3=TREG!F:F), TREG!J:J)</f>
         <v>CAUC</v>
       </c>
     </row>
@@ -46631,7 +46628,7 @@
         <v>1.06</v>
       </c>
       <c r="AP4" s="12" t="str" cm="1">
-        <f t="array" ref="AP4">_xlfn.XLOOKUP(1, (A4=TREG!A:A)*(CU!F4=TREG!F:F), TREG!J:J)</f>
+        <f t="array" aca="1" ref="AP4" ca="1">_xlfn.XLOOKUP(1, (A4=TREG!A:A)*(CU!F4=TREG!F:F), TREG!J:J)</f>
         <v>CAUE</v>
       </c>
     </row>
@@ -46754,7 +46751,7 @@
         <v>0.73699999999999999</v>
       </c>
       <c r="AP5" s="12" t="str" cm="1">
-        <f t="array" ref="AP5">_xlfn.XLOOKUP(1, (A5=TREG!A:A)*(CU!F5=TREG!F:F), TREG!J:J)</f>
+        <f t="array" aca="1" ref="AP5" ca="1">_xlfn.XLOOKUP(1, (A5=TREG!A:A)*(CU!F5=TREG!F:F), TREG!J:J)</f>
         <v>CAUC</v>
       </c>
     </row>
@@ -46877,7 +46874,7 @@
         <v>1.1399999999999999</v>
       </c>
       <c r="AP6" t="str" cm="1">
-        <f t="array" ref="AP6">_xlfn.XLOOKUP(1, (A6=TREG!A:A)*(CU!F6=TREG!F:F), TREG!J:J)</f>
+        <f t="array" aca="1" ref="AP6" ca="1">_xlfn.XLOOKUP(1, (A6=TREG!A:A)*(CU!F6=TREG!F:F), TREG!J:J)</f>
         <v>CAUC</v>
       </c>
     </row>
@@ -47000,7 +46997,7 @@
         <v>0.70099999999999996</v>
       </c>
       <c r="AP7" t="str" cm="1">
-        <f t="array" ref="AP7">_xlfn.XLOOKUP(1, (A7=TREG!A:A)*(CU!F7=TREG!F:F), TREG!J:J)</f>
+        <f t="array" aca="1" ref="AP7" ca="1">_xlfn.XLOOKUP(1, (A7=TREG!A:A)*(CU!F7=TREG!F:F), TREG!J:J)</f>
         <v>CID</v>
       </c>
     </row>
@@ -47123,7 +47120,7 @@
         <v>0.60699999999999998</v>
       </c>
       <c r="AP8" t="str" cm="1">
-        <f t="array" ref="AP8">_xlfn.XLOOKUP(1, (A8=TREG!A:A)*(CU!F8=TREG!F:F), TREG!J:J)</f>
+        <f t="array" aca="1" ref="AP8" ca="1">_xlfn.XLOOKUP(1, (A8=TREG!A:A)*(CU!F8=TREG!F:F), TREG!J:J)</f>
         <v>CID</v>
       </c>
     </row>
@@ -47246,7 +47243,7 @@
         <v>1.01</v>
       </c>
       <c r="AP9" t="str" cm="1">
-        <f t="array" ref="AP9">_xlfn.XLOOKUP(1, (A9=TREG!A:A)*(CU!F9=TREG!F:F), TREG!J:J)</f>
+        <f t="array" aca="1" ref="AP9" ca="1">_xlfn.XLOOKUP(1, (A9=TREG!A:A)*(CU!F9=TREG!F:F), TREG!J:J)</f>
         <v>CAUC</v>
       </c>
     </row>
@@ -47369,7 +47366,7 @@
         <v>1.04</v>
       </c>
       <c r="AP10" t="str" cm="1">
-        <f t="array" ref="AP10">_xlfn.XLOOKUP(1, (A10=TREG!A:A)*(CU!F10=TREG!F:F), TREG!J:J)</f>
+        <f t="array" aca="1" ref="AP10" ca="1">_xlfn.XLOOKUP(1, (A10=TREG!A:A)*(CU!F10=TREG!F:F), TREG!J:J)</f>
         <v>CAUE</v>
       </c>
     </row>
@@ -47615,7 +47612,7 @@
         <v>1.06</v>
       </c>
       <c r="AP12" t="str" cm="1">
-        <f t="array" ref="AP12">_xlfn.XLOOKUP(1, (A12=TREG!A:A)*(CU!F12=TREG!F:F), TREG!J:J)</f>
+        <f t="array" aca="1" ref="AP12" ca="1">_xlfn.XLOOKUP(1, (A12=TREG!A:A)*(CU!F12=TREG!F:F), TREG!J:J)</f>
         <v>CAUE</v>
       </c>
     </row>
@@ -47861,7 +47858,7 @@
         <v>0.53200000000000003</v>
       </c>
       <c r="AP14" t="str" cm="1">
-        <f t="array" ref="AP14">_xlfn.XLOOKUP(1, (A14=TREG!A:A)*(CU!F14=TREG!F:F), TREG!J:J)</f>
+        <f t="array" aca="1" ref="AP14" ca="1">_xlfn.XLOOKUP(1, (A14=TREG!A:A)*(CU!F14=TREG!F:F), TREG!J:J)</f>
         <v>CAUC</v>
       </c>
     </row>
@@ -47984,7 +47981,7 @@
         <v>0.59199999999999997</v>
       </c>
       <c r="AP15" t="str" cm="1">
-        <f t="array" ref="AP15">_xlfn.XLOOKUP(1, (A15=TREG!A:A)*(CU!F15=TREG!F:F), TREG!J:J)</f>
+        <f t="array" aca="1" ref="AP15" ca="1">_xlfn.XLOOKUP(1, (A15=TREG!A:A)*(CU!F15=TREG!F:F), TREG!J:J)</f>
         <v>CAUE</v>
       </c>
     </row>
@@ -48107,7 +48104,7 @@
         <v>0.95</v>
       </c>
       <c r="AP16" t="str" cm="1">
-        <f t="array" ref="AP16">_xlfn.XLOOKUP(1, (A16=TREG!A:A)*(CU!F16=TREG!F:F), TREG!J:J)</f>
+        <f t="array" aca="1" ref="AP16" ca="1">_xlfn.XLOOKUP(1, (A16=TREG!A:A)*(CU!F16=TREG!F:F), TREG!J:J)</f>
         <v>CID</v>
       </c>
     </row>
@@ -48230,7 +48227,7 @@
         <v>0.57699999999999996</v>
       </c>
       <c r="AP17" t="str" cm="1">
-        <f t="array" ref="AP17">_xlfn.XLOOKUP(1, (A17=TREG!A:A)*(CU!F17=TREG!F:F), TREG!J:J)</f>
+        <f t="array" aca="1" ref="AP17" ca="1">_xlfn.XLOOKUP(1, (A17=TREG!A:A)*(CU!F17=TREG!F:F), TREG!J:J)</f>
         <v>CID</v>
       </c>
     </row>
@@ -48599,7 +48596,7 @@
         <v>1.05</v>
       </c>
       <c r="AP20" t="str" cm="1">
-        <f t="array" ref="AP20">_xlfn.XLOOKUP(1, (A20=TREG!A:A)*(CU!F20=TREG!F:F), TREG!J:J)</f>
+        <f t="array" aca="1" ref="AP20" ca="1">_xlfn.XLOOKUP(1, (A20=TREG!A:A)*(CU!F20=TREG!F:F), TREG!J:J)</f>
         <v>CIU</v>
       </c>
     </row>
@@ -48845,7 +48842,7 @@
         <v>0.70299999999999996</v>
       </c>
       <c r="AP22" t="str" cm="1">
-        <f t="array" ref="AP22">_xlfn.XLOOKUP(1, (A22=TREG!A:A)*(CU!F22=TREG!F:F), TREG!J:J)</f>
+        <f t="array" aca="1" ref="AP22" ca="1">_xlfn.XLOOKUP(1, (A22=TREG!A:A)*(CU!F22=TREG!F:F), TREG!J:J)</f>
         <v>CIU</v>
       </c>
     </row>
@@ -49091,7 +49088,7 @@
         <v>0.94399999999999995</v>
       </c>
       <c r="AP24" t="str" cm="1">
-        <f t="array" ref="AP24">_xlfn.XLOOKUP(1, (A24=TREG!A:A)*(CU!F24=TREG!F:F), TREG!J:J)</f>
+        <f t="array" aca="1" ref="AP24" ca="1">_xlfn.XLOOKUP(1, (A24=TREG!A:A)*(CU!F24=TREG!F:F), TREG!J:J)</f>
         <v>CAUC</v>
       </c>
     </row>
@@ -49337,7 +49334,7 @@
         <v>0.70599999999999996</v>
       </c>
       <c r="AP26" t="str" cm="1">
-        <f t="array" ref="AP26">_xlfn.XLOOKUP(1, (A26=TREG!A:A)*(CU!F26=TREG!F:F), TREG!J:J)</f>
+        <f t="array" aca="1" ref="AP26" ca="1">_xlfn.XLOOKUP(1, (A26=TREG!A:A)*(CU!F26=TREG!F:F), TREG!J:J)</f>
         <v>CID</v>
       </c>
     </row>
@@ -49583,7 +49580,7 @@
         <v>0.65400000000000003</v>
       </c>
       <c r="AP28" t="str" cm="1">
-        <f t="array" ref="AP28">_xlfn.XLOOKUP(1, (A28=TREG!A:A)*(CU!F28=TREG!F:F), TREG!J:J)</f>
+        <f t="array" aca="1" ref="AP28" ca="1">_xlfn.XLOOKUP(1, (A28=TREG!A:A)*(CU!F28=TREG!F:F), TREG!J:J)</f>
         <v>CID</v>
       </c>
     </row>
@@ -49829,7 +49826,7 @@
         <v>0.78</v>
       </c>
       <c r="AP30" t="str" cm="1">
-        <f t="array" ref="AP30">_xlfn.XLOOKUP(1, (A30=TREG!A:A)*(CU!F30=TREG!F:F), TREG!J:J)</f>
+        <f t="array" aca="1" ref="AP30" ca="1">_xlfn.XLOOKUP(1, (A30=TREG!A:A)*(CU!F30=TREG!F:F), TREG!J:J)</f>
         <v>CIU</v>
       </c>
     </row>
@@ -50075,7 +50072,7 @@
         <v>0.58499999999999996</v>
       </c>
       <c r="AP32" t="str" cm="1">
-        <f t="array" ref="AP32">_xlfn.XLOOKUP(1, (A32=TREG!A:A)*(CU!F32=TREG!F:F), TREG!J:J)</f>
+        <f t="array" aca="1" ref="AP32" ca="1">_xlfn.XLOOKUP(1, (A32=TREG!A:A)*(CU!F32=TREG!F:F), TREG!J:J)</f>
         <v>CID</v>
       </c>
     </row>
@@ -50321,7 +50318,7 @@
         <v>0.94799999999999995</v>
       </c>
       <c r="AP34" t="str" cm="1">
-        <f t="array" ref="AP34">_xlfn.XLOOKUP(1, (A34=TREG!A:A)*(CU!F34=TREG!F:F), TREG!J:J)</f>
+        <f t="array" aca="1" ref="AP34" ca="1">_xlfn.XLOOKUP(1, (A34=TREG!A:A)*(CU!F34=TREG!F:F), TREG!J:J)</f>
         <v>CAUC</v>
       </c>
     </row>
@@ -50567,7 +50564,7 @@
         <v>0.83699999999999997</v>
       </c>
       <c r="AP36" t="str" cm="1">
-        <f t="array" ref="AP36">_xlfn.XLOOKUP(1, (A36=TREG!A:A)*(CU!F36=TREG!F:F), TREG!J:J)</f>
+        <f t="array" aca="1" ref="AP36" ca="1">_xlfn.XLOOKUP(1, (A36=TREG!A:A)*(CU!F36=TREG!F:F), TREG!J:J)</f>
         <v>CID</v>
       </c>
     </row>
@@ -50813,7 +50810,7 @@
         <v>0.80800000000000005</v>
       </c>
       <c r="AP38" t="str" cm="1">
-        <f t="array" ref="AP38">_xlfn.XLOOKUP(1, (A38=TREG!A:A)*(CU!F38=TREG!F:F), TREG!J:J)</f>
+        <f t="array" aca="1" ref="AP38" ca="1">_xlfn.XLOOKUP(1, (A38=TREG!A:A)*(CU!F38=TREG!F:F), TREG!J:J)</f>
         <v>CID</v>
       </c>
     </row>
@@ -51059,7 +51056,7 @@
         <v>0.69199999999999995</v>
       </c>
       <c r="AP40" t="str" cm="1">
-        <f t="array" ref="AP40">_xlfn.XLOOKUP(1, (A40=TREG!A:A)*(CU!F40=TREG!F:F), TREG!J:J)</f>
+        <f t="array" aca="1" ref="AP40" ca="1">_xlfn.XLOOKUP(1, (A40=TREG!A:A)*(CU!F40=TREG!F:F), TREG!J:J)</f>
         <v>CIU</v>
       </c>
     </row>
@@ -51305,7 +51302,7 @@
         <v>0.94799999999999995</v>
       </c>
       <c r="AP42" t="str" cm="1">
-        <f t="array" ref="AP42">_xlfn.XLOOKUP(1, (A42=TREG!A:A)*(CU!F42=TREG!F:F), TREG!J:J)</f>
+        <f t="array" aca="1" ref="AP42" ca="1">_xlfn.XLOOKUP(1, (A42=TREG!A:A)*(CU!F42=TREG!F:F), TREG!J:J)</f>
         <v>CID</v>
       </c>
     </row>
@@ -51551,7 +51548,7 @@
         <v>0.499</v>
       </c>
       <c r="AP44" t="str" cm="1">
-        <f t="array" ref="AP44">_xlfn.XLOOKUP(1, (A44=TREG!A:A)*(CU!F44=TREG!F:F), TREG!J:J)</f>
+        <f t="array" aca="1" ref="AP44" ca="1">_xlfn.XLOOKUP(1, (A44=TREG!A:A)*(CU!F44=TREG!F:F), TREG!J:J)</f>
         <v>CID</v>
       </c>
     </row>
@@ -51797,7 +51794,7 @@
         <v>0.63900000000000001</v>
       </c>
       <c r="AP46" t="str" cm="1">
-        <f t="array" ref="AP46">_xlfn.XLOOKUP(1, (A46=TREG!A:A)*(CU!F46=TREG!F:F), TREG!J:J)</f>
+        <f t="array" aca="1" ref="AP46" ca="1">_xlfn.XLOOKUP(1, (A46=TREG!A:A)*(CU!F46=TREG!F:F), TREG!J:J)</f>
         <v>CIU</v>
       </c>
     </row>
@@ -52043,7 +52040,7 @@
         <v>0.71699999999999997</v>
       </c>
       <c r="AP48" t="str" cm="1">
-        <f t="array" ref="AP48">_xlfn.XLOOKUP(1, (A48=TREG!A:A)*(CU!F48=TREG!F:F), TREG!J:J)</f>
+        <f t="array" aca="1" ref="AP48" ca="1">_xlfn.XLOOKUP(1, (A48=TREG!A:A)*(CU!F48=TREG!F:F), TREG!J:J)</f>
         <v>CAUC</v>
       </c>
     </row>
@@ -52166,7 +52163,7 @@
         <v>0.746</v>
       </c>
       <c r="AP49" t="str" cm="1">
-        <f t="array" ref="AP49">_xlfn.XLOOKUP(1, (A49=TREG!A:A)*(CU!F49=TREG!F:F), TREG!J:J)</f>
+        <f t="array" aca="1" ref="AP49" ca="1">_xlfn.XLOOKUP(1, (A49=TREG!A:A)*(CU!F49=TREG!F:F), TREG!J:J)</f>
         <v>CAUC</v>
       </c>
     </row>
@@ -52289,7 +52286,7 @@
         <v>0.73399999999999999</v>
       </c>
       <c r="AP50" t="str" cm="1">
-        <f t="array" ref="AP50">_xlfn.XLOOKUP(1, (A50=TREG!A:A)*(CU!F50=TREG!F:F), TREG!J:J)</f>
+        <f t="array" aca="1" ref="AP50" ca="1">_xlfn.XLOOKUP(1, (A50=TREG!A:A)*(CU!F50=TREG!F:F), TREG!J:J)</f>
         <v>CAUE</v>
       </c>
     </row>
@@ -52535,7 +52532,7 @@
         <v>0.77300000000000002</v>
       </c>
       <c r="AP52" t="str" cm="1">
-        <f t="array" ref="AP52">_xlfn.XLOOKUP(1, (A52=TREG!A:A)*(CU!F52=TREG!F:F), TREG!J:J)</f>
+        <f t="array" aca="1" ref="AP52" ca="1">_xlfn.XLOOKUP(1, (A52=TREG!A:A)*(CU!F52=TREG!F:F), TREG!J:J)</f>
         <v>CAUC</v>
       </c>
     </row>
@@ -52781,7 +52778,7 @@
         <v>0.68200000000000005</v>
       </c>
       <c r="AP54" t="str" cm="1">
-        <f t="array" ref="AP54">_xlfn.XLOOKUP(1, (A54=TREG!A:A)*(CU!F54=TREG!F:F), TREG!J:J)</f>
+        <f t="array" aca="1" ref="AP54" ca="1">_xlfn.XLOOKUP(1, (A54=TREG!A:A)*(CU!F54=TREG!F:F), TREG!J:J)</f>
         <v>CID</v>
       </c>
     </row>
@@ -52904,7 +52901,7 @@
         <v>0.77</v>
       </c>
       <c r="AP55" t="str" cm="1">
-        <f t="array" ref="AP55">_xlfn.XLOOKUP(1, (A55=TREG!A:A)*(CU!F55=TREG!F:F), TREG!J:J)</f>
+        <f t="array" aca="1" ref="AP55" ca="1">_xlfn.XLOOKUP(1, (A55=TREG!A:A)*(CU!F55=TREG!F:F), TREG!J:J)</f>
         <v>CID</v>
       </c>
     </row>
@@ -53027,7 +53024,7 @@
         <v>0.92200000000000004</v>
       </c>
       <c r="AP56" t="str" cm="1">
-        <f t="array" ref="AP56">_xlfn.XLOOKUP(1, (A56=TREG!A:A)*(CU!F56=TREG!F:F), TREG!J:J)</f>
+        <f t="array" aca="1" ref="AP56" ca="1">_xlfn.XLOOKUP(1, (A56=TREG!A:A)*(CU!F56=TREG!F:F), TREG!J:J)</f>
         <v>CID</v>
       </c>
     </row>
@@ -53150,7 +53147,7 @@
         <v>0.68700000000000006</v>
       </c>
       <c r="AP57" t="str" cm="1">
-        <f t="array" ref="AP57">_xlfn.XLOOKUP(1, (A57=TREG!A:A)*(CU!F57=TREG!F:F), TREG!J:J)</f>
+        <f t="array" aca="1" ref="AP57" ca="1">_xlfn.XLOOKUP(1, (A57=TREG!A:A)*(CU!F57=TREG!F:F), TREG!J:J)</f>
         <v>CID</v>
       </c>
     </row>
@@ -53273,7 +53270,7 @@
         <v>0.65500000000000003</v>
       </c>
       <c r="AP58" t="str" cm="1">
-        <f t="array" ref="AP58">_xlfn.XLOOKUP(1, (A58=TREG!A:A)*(CU!F58=TREG!F:F), TREG!J:J)</f>
+        <f t="array" aca="1" ref="AP58" ca="1">_xlfn.XLOOKUP(1, (A58=TREG!A:A)*(CU!F58=TREG!F:F), TREG!J:J)</f>
         <v>CID</v>
       </c>
     </row>
@@ -53519,7 +53516,7 @@
         <v>0.96799999999999997</v>
       </c>
       <c r="AP60" t="str" cm="1">
-        <f t="array" ref="AP60">_xlfn.XLOOKUP(1, (A60=TREG!A:A)*(CU!F60=TREG!F:F), TREG!J:J)</f>
+        <f t="array" aca="1" ref="AP60" ca="1">_xlfn.XLOOKUP(1, (A60=TREG!A:A)*(CU!F60=TREG!F:F), TREG!J:J)</f>
         <v>CAUC</v>
       </c>
     </row>
@@ -53642,7 +53639,7 @@
         <v>1.5</v>
       </c>
       <c r="AP61" t="str" cm="1">
-        <f t="array" ref="AP61">_xlfn.XLOOKUP(1, (A61=TREG!A:A)*(CU!F61=TREG!F:F), TREG!J:J)</f>
+        <f t="array" aca="1" ref="AP61" ca="1">_xlfn.XLOOKUP(1, (A61=TREG!A:A)*(CU!F61=TREG!F:F), TREG!J:J)</f>
         <v>CIU</v>
       </c>
     </row>
@@ -53765,7 +53762,7 @@
         <v>0.69</v>
       </c>
       <c r="AP62" t="str" cm="1">
-        <f t="array" ref="AP62">_xlfn.XLOOKUP(1, (A62=TREG!A:A)*(CU!F62=TREG!F:F), TREG!J:J)</f>
+        <f t="array" aca="1" ref="AP62" ca="1">_xlfn.XLOOKUP(1, (A62=TREG!A:A)*(CU!F62=TREG!F:F), TREG!J:J)</f>
         <v>CID</v>
       </c>
     </row>
@@ -53888,7 +53885,7 @@
         <v>0.60699999999999998</v>
       </c>
       <c r="AP63" t="str" cm="1">
-        <f t="array" ref="AP63">_xlfn.XLOOKUP(1, (A63=TREG!A:A)*(CU!F63=TREG!F:F), TREG!J:J)</f>
+        <f t="array" aca="1" ref="AP63" ca="1">_xlfn.XLOOKUP(1, (A63=TREG!A:A)*(CU!F63=TREG!F:F), TREG!J:J)</f>
         <v>CID</v>
       </c>
     </row>
@@ -54011,7 +54008,7 @@
         <v>0.55000000000000004</v>
       </c>
       <c r="AP64" t="str" cm="1">
-        <f t="array" ref="AP64">_xlfn.XLOOKUP(1, (A64=TREG!A:A)*(CU!F64=TREG!F:F), TREG!J:J)</f>
+        <f t="array" aca="1" ref="AP64" ca="1">_xlfn.XLOOKUP(1, (A64=TREG!A:A)*(CU!F64=TREG!F:F), TREG!J:J)</f>
         <v>CID</v>
       </c>
     </row>
@@ -54257,7 +54254,7 @@
         <v>0.93200000000000005</v>
       </c>
       <c r="AP66" t="str" cm="1">
-        <f t="array" ref="AP66">_xlfn.XLOOKUP(1, (A66=TREG!A:A)*(CU!F66=TREG!F:F), TREG!J:J)</f>
+        <f t="array" aca="1" ref="AP66" ca="1">_xlfn.XLOOKUP(1, (A66=TREG!A:A)*(CU!F66=TREG!F:F), TREG!J:J)</f>
         <v>CIU</v>
       </c>
     </row>
@@ -54380,7 +54377,7 @@
         <v>0.56100000000000005</v>
       </c>
       <c r="AP67" t="str" cm="1">
-        <f t="array" ref="AP67">_xlfn.XLOOKUP(1, (A67=TREG!A:A)*(CU!F67=TREG!F:F), TREG!J:J)</f>
+        <f t="array" aca="1" ref="AP67" ca="1">_xlfn.XLOOKUP(1, (A67=TREG!A:A)*(CU!F67=TREG!F:F), TREG!J:J)</f>
         <v>CID</v>
       </c>
     </row>
@@ -54503,7 +54500,7 @@
         <v>0.74199999999999999</v>
       </c>
       <c r="AP68" t="str" cm="1">
-        <f t="array" ref="AP68">_xlfn.XLOOKUP(1, (A68=TREG!A:A)*(CU!F68=TREG!F:F), TREG!J:J)</f>
+        <f t="array" aca="1" ref="AP68" ca="1">_xlfn.XLOOKUP(1, (A68=TREG!A:A)*(CU!F68=TREG!F:F), TREG!J:J)</f>
         <v>CAUC</v>
       </c>
     </row>
@@ -54626,7 +54623,7 @@
         <v>0.77600000000000002</v>
       </c>
       <c r="AP69" t="str" cm="1">
-        <f t="array" ref="AP69">_xlfn.XLOOKUP(1, (A69=TREG!A:A)*(CU!F69=TREG!F:F), TREG!J:J)</f>
+        <f t="array" aca="1" ref="AP69" ca="1">_xlfn.XLOOKUP(1, (A69=TREG!A:A)*(CU!F69=TREG!F:F), TREG!J:J)</f>
         <v>CAUE</v>
       </c>
     </row>
@@ -54749,7 +54746,7 @@
         <v>1.04</v>
       </c>
       <c r="AP70" t="str" cm="1">
-        <f t="array" ref="AP70">_xlfn.XLOOKUP(1, (A70=TREG!A:A)*(CU!F70=TREG!F:F), TREG!J:J)</f>
+        <f t="array" aca="1" ref="AP70" ca="1">_xlfn.XLOOKUP(1, (A70=TREG!A:A)*(CU!F70=TREG!F:F), TREG!J:J)</f>
         <v>CIU</v>
       </c>
     </row>
@@ -54872,7 +54869,7 @@
         <v>0.68500000000000005</v>
       </c>
       <c r="AP71" t="str" cm="1">
-        <f t="array" ref="AP71">_xlfn.XLOOKUP(1, (A71=TREG!A:A)*(CU!F71=TREG!F:F), TREG!J:J)</f>
+        <f t="array" aca="1" ref="AP71" ca="1">_xlfn.XLOOKUP(1, (A71=TREG!A:A)*(CU!F71=TREG!F:F), TREG!J:J)</f>
         <v>CIU</v>
       </c>
     </row>
@@ -54995,7 +54992,7 @@
         <v>1.25</v>
       </c>
       <c r="AP72" t="str" cm="1">
-        <f t="array" ref="AP72">_xlfn.XLOOKUP(1, (A72=TREG!A:A)*(CU!F72=TREG!F:F), TREG!J:J)</f>
+        <f t="array" aca="1" ref="AP72" ca="1">_xlfn.XLOOKUP(1, (A72=TREG!A:A)*(CU!F72=TREG!F:F), TREG!J:J)</f>
         <v>CAUC</v>
       </c>
     </row>
@@ -55118,7 +55115,7 @@
         <v>1.28</v>
       </c>
       <c r="AP73" t="str" cm="1">
-        <f t="array" ref="AP73">_xlfn.XLOOKUP(1, (A73=TREG!A:A)*(CU!F73=TREG!F:F), TREG!J:J)</f>
+        <f t="array" aca="1" ref="AP73" ca="1">_xlfn.XLOOKUP(1, (A73=TREG!A:A)*(CU!F73=TREG!F:F), TREG!J:J)</f>
         <v>CAUE</v>
       </c>
     </row>
@@ -55241,7 +55238,7 @@
         <v>1.1100000000000001</v>
       </c>
       <c r="AP74" t="str" cm="1">
-        <f t="array" ref="AP74">_xlfn.XLOOKUP(1, (A74=TREG!A:A)*(CU!F74=TREG!F:F), TREG!J:J)</f>
+        <f t="array" aca="1" ref="AP74" ca="1">_xlfn.XLOOKUP(1, (A74=TREG!A:A)*(CU!F74=TREG!F:F), TREG!J:J)</f>
         <v>CIU</v>
       </c>
     </row>

</xml_diff>